<commit_message>
Ultimo push antes de la ultima entrega
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edu\Desktop\Programanding\2do Año\MP13 Projecte\WanderingShadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86098F2-66AE-4CA6-A61D-07883FBE2DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F6E25C-D8DA-4598-B627-AEBF7F9CD4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C7E29CD0-FBB8-43D8-85F7-7A854540FE63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -152,6 +152,24 @@
   </si>
   <si>
     <t>Si</t>
+  </si>
+  <si>
+    <t>Animacion How To Play</t>
+  </si>
+  <si>
+    <t>Algunos botones del how to play tienen animaciones que en otra escena no se reproducen</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>El samurai tiene extra doble salto</t>
+  </si>
+  <si>
+    <t>Cuando el samurai se queda un segundo pegado de una saliente, se reinicia su contar de salto, por lo cual puede saltar dos veces otra vez aun cayendo</t>
   </si>
 </sst>
 </file>
@@ -530,13 +548,13 @@
   <dimension ref="C6:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="11" max="11" width="33.7109375" customWidth="1"/>
@@ -723,11 +741,38 @@
       <c r="C12">
         <v>6</v>
       </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>7</v>
       </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -736,6 +781,9 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -744,6 +792,9 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -752,6 +803,9 @@
       <c r="D16" t="s">
         <v>29</v>
       </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17">
@@ -760,6 +814,12 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18">
@@ -768,6 +828,15 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19">
@@ -776,6 +845,12 @@
       <c r="D19" t="s">
         <v>32</v>
       </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="L19" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20">
@@ -784,6 +859,15 @@
       <c r="D20" t="s">
         <v>33</v>
       </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21">
@@ -792,6 +876,9 @@
       <c r="D21" t="s">
         <v>34</v>
       </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C22">
@@ -800,8 +887,8 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="L22" t="s">
-        <v>38</v>
+      <c r="G22">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
@@ -809,7 +896,10 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">

</xml_diff>